<commit_message>
begin incorporating google sheets
</commit_message>
<xml_diff>
--- a/shiny_application/global/database/jobs.xlsx
+++ b/shiny_application/global/database/jobs.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr date1904="false"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
@@ -26,13 +26,13 @@
     <t xml:space="preserve">[{"job_id":2,"customer":"Kerry","site":"6 Cliff Parade","cs_number":"321","dwg_number":"654","start_date":19158,"required_by":19173,"hours_mill":5,"hours_program":0,"hours_cnc":0,"hours_veneer":10,"hours_bench":10,"hours_spray":10,"hours_dispatch":1,"active":1,"created_by":"a117644@r02.xlgs.local","created_on":"2022-06-13 16:00:50","updated_by":"a117644@r02.xlgs.local","updated_on":"2022-06-13 16:00:50","start_date_mill":19158,"days_mill":1,"end_date_mill":19163,"start_date_program":19163,"days_program":0,"end_date_program":19163,"start_date_cnc":19163,"days_cnc":0,"end_date_cnc":19163,"start_date_veneer":19163,"days_veneer":2,"end_date_veneer":19165,"start_date_bench":19165,"days_bench":2,"end_date_bench":19167,"start_date_spray":19167,"days_spray":2,"end_date_spray":19171,"start_date_dispatch":19171,"days_dispatch":1,"end_date_dispatch":19172,"days_overrun":0,"start_date_recommended":19158}]</t>
   </si>
   <si>
-    <t xml:space="preserve">[{"job_id":3,"customer":"Alex","site":"Brighton Avenue","cs_number":"666","dwg_number":"0","start_date":19180,"required_by":19208,"hours_mill":25,"hours_program":10,"hours_cnc":20,"hours_veneer":0,"hours_bench":10,"hours_spray":0,"hours_dispatch":1,"active":1,"created_by":"a117644@r02.xlgs.local","created_on":"2022-07-07 17:37:37","updated_by":"a117644@r02.xlgs.local","updated_on":"2022-07-07 17:37:37","start_date_mill":19180,"days_mill":4,"end_date_mill":19186,"start_date_program":19186,"days_program":2,"end_date_program":19188,"start_date_cnc":19188,"days_cnc":3,"end_date_cnc":19193,"start_date_veneer":19193,"days_veneer":0,"end_date_veneer":19193,"start_date_bench":19193,"days_bench":2,"end_date_bench":19195,"start_date_spray":19195,"days_spray":0,"end_date_spray":19195,"start_date_dispatch":19195,"days_dispatch":1,"end_date_dispatch":19198,"days_overrun":0,"start_date_recommended":19180}]</t>
+    <t xml:space="preserve">[{"job_id":3,"customer":"Alex","site":"Brighton Avenue","cs_number":"666","dwg_number":"0","start_date":19180,"required_by":19208,"hours_mill":25,"hours_program":10,"hours_cnc":20,"hours_veneer":0,"hours_bench":10,"hours_spray":0,"hours_dispatch":1,"active":0,"created_by":"a117644@r02.xlgs.local","created_on":"2022-07-07 17:37:37","updated_by":"a117644@r02.xlgs.local","updated_on":"2022-07-07 17:37:37","start_date_mill":19180,"days_mill":4,"end_date_mill":19186,"start_date_program":19186,"days_program":2,"end_date_program":19188,"start_date_cnc":19188,"days_cnc":3,"end_date_cnc":19193,"start_date_veneer":19193,"days_veneer":0,"end_date_veneer":19193,"start_date_bench":19193,"days_bench":2,"end_date_bench":19195,"start_date_spray":19195,"days_spray":0,"end_date_spray":19195,"start_date_dispatch":19195,"days_dispatch":1,"end_date_dispatch":19198,"days_overrun":0,"start_date_recommended":19180}]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
   <fonts count="1">
     <font>
@@ -351,12 +351,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="1"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
@@ -387,6 +387,14 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>